<commit_message>
added Javadoc comments to provide clear overview of each class and tests
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -44,7 +44,7 @@
     <t>SiriusBond</t>
   </si>
   <si>
-    <t xml:space="preserve">TealBond </t>
+    <t>TealBond</t>
   </si>
   <si>
     <t>JasmineBond</t>
@@ -62,7 +62,7 @@
     <t>LilyBond</t>
   </si>
   <si>
-    <t>OrchidBond</t>
+    <t>OrchidStock</t>
   </si>
   <si>
     <t>DaisyStock</t>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>SaiphStock</t>
+  </si>
+  <si>
+    <t>DIHStock</t>
+  </si>
+  <si>
+    <t>CoupBond</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -176,7 +182,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>80.0</v>
+        <v>90.0</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>110.0</v>
@@ -185,7 +191,7 @@
         <v>115.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>400.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="3">
@@ -379,13 +385,13 @@
         <v>120.0</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>1000.0</v>
+        <v>110.0</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>995.0</v>
+        <v>115.0</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>-600.0</v>
+        <v>600.0</v>
       </c>
     </row>
     <row r="13">
@@ -566,6 +572,46 @@
       </c>
       <c r="F21" t="n" s="0">
         <v>325.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C22" t="n" s="0">
+        <v>53.0</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E22" t="n" s="0">
+        <v>110.0</v>
+      </c>
+      <c r="F22" t="n" s="0">
+        <v>530.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C23" t="n" s="0">
+        <v>75.0</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>850.0</v>
+      </c>
+      <c r="E23" t="n" s="0">
+        <v>1050.0</v>
+      </c>
+      <c r="F23" t="n" s="0">
+        <v>15000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new investment validation exceptions
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -38,15 +38,15 @@
     <t>GlueStock</t>
   </si>
   <si>
+    <t>GovBond</t>
+  </si>
+  <si>
     <t>VegaStock</t>
   </si>
   <si>
     <t>SiriusBond</t>
   </si>
   <si>
-    <t>TealBond</t>
-  </si>
-  <si>
     <t>JasmineBond</t>
   </si>
   <si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>TulipStock</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
   <si>
     <t>LilyBond</t>
@@ -140,7 +137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -216,62 +213,62 @@
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>3.0</v>
+        <v>34.0</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>60.0</v>
+        <v>12.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>150.0</v>
+        <v>6.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>155.0</v>
+        <v>12.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>300.0</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>70.0</v>
+        <v>60.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>180.0</v>
+        <v>150.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>185.0</v>
+        <v>155.0</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>350.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>10</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>23.0</v>
+        <v>70.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>65.0</v>
+        <v>180.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>89.0</v>
+        <v>185.0</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>552.0</v>
+        <v>350.0</v>
       </c>
     </row>
     <row r="7">
@@ -336,281 +333,261 @@
     </row>
     <row r="10">
       <c r="A10" t="n" s="0">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>34.0</v>
+        <v>70.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>65.0</v>
+        <v>200.0</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>78.0</v>
+        <v>205.0</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>442.0</v>
+        <v>350.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n" s="0">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B11" t="s" s="0">
         <v>15</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>70.0</v>
+        <v>120.0</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>200.0</v>
+        <v>110.0</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>205.0</v>
+        <v>115.0</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>350.0</v>
+        <v>600.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n" s="0">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>16</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>120.0</v>
+        <v>95.0</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>110.0</v>
+        <v>220.0</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>115.0</v>
+        <v>225.0</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>600.0</v>
+        <v>475.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n" s="0">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="B13" t="s" s="0">
         <v>17</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>95.0</v>
+        <v>50.0</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>220.0</v>
+        <v>150.0</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>225.0</v>
+        <v>155.0</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>475.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n" s="0">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="B14" t="s" s="0">
         <v>18</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>50.0</v>
+        <v>65.0</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>150.0</v>
+        <v>180.0</v>
       </c>
       <c r="E14" t="n" s="0">
-        <v>155.0</v>
+        <v>185.0</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>250.0</v>
+        <v>325.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n" s="0">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="B15" t="s" s="0">
         <v>19</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>65.0</v>
+        <v>55.0</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>180.0</v>
+        <v>170.0</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>185.0</v>
+        <v>175.0</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>325.0</v>
+        <v>275.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n" s="0">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="B16" t="s" s="0">
         <v>20</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>55.0</v>
+        <v>40.0</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>170.0</v>
+        <v>160.0</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>175.0</v>
+        <v>165.0</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>275.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n" s="0">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>21</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>40.0</v>
+        <v>75.0</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>160.0</v>
+        <v>230.0</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>165.0</v>
+        <v>235.0</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>200.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n" s="0">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>22</v>
       </c>
       <c r="C18" t="n" s="0">
-        <v>75.0</v>
+        <v>60.0</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>230.0</v>
+        <v>250.0</v>
       </c>
       <c r="E18" t="n" s="0">
-        <v>235.0</v>
+        <v>255.0</v>
       </c>
       <c r="F18" t="n" s="0">
-        <v>375.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n" s="0">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="B19" t="s" s="0">
         <v>23</v>
       </c>
       <c r="C19" t="n" s="0">
-        <v>60.0</v>
+        <v>85.0</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>250.0</v>
+        <v>240.0</v>
       </c>
       <c r="E19" t="n" s="0">
-        <v>255.0</v>
+        <v>245.0</v>
       </c>
       <c r="F19" t="n" s="0">
-        <v>300.0</v>
+        <v>425.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n" s="0">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="B20" t="s" s="0">
         <v>24</v>
       </c>
       <c r="C20" t="n" s="0">
-        <v>85.0</v>
+        <v>65.0</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>240.0</v>
+        <v>260.0</v>
       </c>
       <c r="E20" t="n" s="0">
-        <v>245.0</v>
+        <v>265.0</v>
       </c>
       <c r="F20" t="n" s="0">
-        <v>425.0</v>
+        <v>325.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n" s="0">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="B21" t="s" s="0">
         <v>25</v>
       </c>
       <c r="C21" t="n" s="0">
-        <v>65.0</v>
+        <v>53.0</v>
       </c>
       <c r="D21" t="n" s="0">
-        <v>260.0</v>
+        <v>100.0</v>
       </c>
       <c r="E21" t="n" s="0">
-        <v>265.0</v>
+        <v>110.0</v>
       </c>
       <c r="F21" t="n" s="0">
-        <v>325.0</v>
+        <v>530.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n" s="0">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>26</v>
       </c>
       <c r="C22" t="n" s="0">
-        <v>53.0</v>
+        <v>75.0</v>
       </c>
       <c r="D22" t="n" s="0">
-        <v>100.0</v>
+        <v>1000.0</v>
       </c>
       <c r="E22" t="n" s="0">
-        <v>110.0</v>
+        <v>1050.0</v>
       </c>
       <c r="F22" t="n" s="0">
-        <v>530.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n" s="0">
-        <v>23.0</v>
-      </c>
-      <c r="B23" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="C23" t="n" s="0">
-        <v>75.0</v>
-      </c>
-      <c r="D23" t="n" s="0">
-        <v>1000.0</v>
-      </c>
-      <c r="E23" t="n" s="0">
-        <v>1050.0</v>
-      </c>
-      <c r="F23" t="n" s="0">
         <v>3750.0</v>
       </c>
     </row>

</xml_diff>